<commit_message>
new unit test for peak coolant temp incl full dassh calc; bug fixes in orificing.py; cleanup handcalc spreadsheet
</commit_message>
<xml_diff>
--- a/tests/test_data/orificing-1/hand_calculation.xlsx
+++ b/tests/test_data/orificing-1/hand_calculation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matz/Documents/DASSH/Analysis/orificing/unit_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matz/Documents/DASSH/src_DASSH/tests/test_data/orificing-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22199402-ABAA-ED4D-8954-A6726B575F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C3506E-E0A4-3043-B421-793F2D86074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="3" xr2:uid="{ECDE5AF7-12FD-C942-A9DC-96DDFD800A19}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="iter-2 setup" sheetId="3" r:id="rId3"/>
     <sheet name="iter-3 setup (converged)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="69">
   <si>
     <t>Asm ID</t>
   </si>
@@ -275,7 +275,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -336,7 +336,7 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -752,14 +752,14 @@
         <v>13840.3332953751</v>
       </c>
       <c r="G7" s="4">
-        <f>(D7-E7)/F7</f>
+        <f t="shared" ref="G7:G25" si="0">(D7-E7)/F7</f>
         <v>0</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
       </c>
       <c r="I7" s="3">
-        <f>IF(G7&gt;B$2, 1, 0)</f>
+        <f t="shared" ref="I7:I25" si="1">IF(G7&gt;B$2, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="J7" s="3">
@@ -793,7 +793,7 @@
         <v>13157.623186377201</v>
       </c>
       <c r="G8" s="4">
-        <f ca="1">(D8-E8)/F8</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.10377407824001926</v>
       </c>
       <c r="H8" s="3">
@@ -801,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="3">
-        <f ca="1">IF(G8&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J8" s="3">
@@ -809,7 +809,7 @@
         <v>1</v>
       </c>
       <c r="K8" t="str">
-        <f ca="1">IF(I8=0, K7, ADDRESS(H8+7,3))</f>
+        <f t="shared" ref="K8:K25" ca="1" si="2">IF(I8=0, K7, ADDRESS(H8+7,3))</f>
         <v>$C$7</v>
       </c>
     </row>
@@ -836,23 +836,23 @@
         <v>12930.053150044567</v>
       </c>
       <c r="G9" s="4">
-        <f ca="1">(D9-E9)/F9</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.10560051085258633</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" ref="H9:H25" si="0">H8+1</f>
+        <f t="shared" ref="H9:H25" si="3">H8+1</f>
         <v>3</v>
       </c>
       <c r="I9" s="3">
-        <f ca="1">IF(G9&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" ref="J9:J25" ca="1" si="1">I9+J8</f>
+        <f t="shared" ref="J9:J25" ca="1" si="4">I9+J8</f>
         <v>1</v>
       </c>
       <c r="K9" t="str">
-        <f ca="1">IF(I9=0, K8, ADDRESS(H9+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$7</v>
       </c>
     </row>
@@ -879,23 +879,23 @@
         <v>12816.268131878251</v>
       </c>
       <c r="G10" s="4">
-        <f ca="1">(D10-E10)/F10</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.10653805023004728</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="I10" s="3">
-        <f ca="1">IF(G10&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="K10" t="str">
-        <f ca="1">IF(I10=0, K9, ADDRESS(H10+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$7</v>
       </c>
     </row>
@@ -922,23 +922,23 @@
         <v>12747.996700068201</v>
       </c>
       <c r="G11" s="4">
-        <f ca="1">(D11-E11)/F11</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.10710877596475959</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="I11" s="3">
-        <f ca="1">IF(G11&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="K11" t="str">
-        <f ca="1">IF(I11=0, K10, ADDRESS(H11+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$7</v>
       </c>
     </row>
@@ -965,23 +965,23 @@
         <v>12702.482412194833</v>
       </c>
       <c r="G12" s="4">
-        <f ca="1">(D12-E12)/F12</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.10749255761505687</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="I12" s="3">
-        <f ca="1">IF(G12&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="K12" t="str">
-        <f ca="1">IF(I12=0, K11, ADDRESS(H12+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$7</v>
       </c>
     </row>
@@ -1008,23 +1008,23 @@
         <v>12669.972206570999</v>
       </c>
       <c r="G13" s="4">
-        <f ca="1">(D13-E13)/F13</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.10776837551695288</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="I13" s="3">
-        <f ca="1">IF(G13&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>1</v>
       </c>
       <c r="K13" t="str">
-        <f ca="1">IF(I13=0, K12, ADDRESS(H13+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$7</v>
       </c>
     </row>
@@ -1051,23 +1051,23 @@
         <v>12435.216841134763</v>
       </c>
       <c r="G14" s="4">
-        <f ca="1">(D14-E14)/F14</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.24514281103728799</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I14" s="3">
-        <f ca="1">IF(G14&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="K14" t="str">
-        <f ca="1">IF(I14=0, K13, ADDRESS(H14+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$15</v>
       </c>
     </row>
@@ -1094,23 +1094,23 @@
         <v>10791.929283081099</v>
       </c>
       <c r="G15" s="4">
-        <f ca="1">(D15-E15)/F15</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="I15" s="3">
-        <f ca="1">IF(G15&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="K15" t="str">
-        <f ca="1">IF(I15=0, K14, ADDRESS(H15+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$15</v>
       </c>
     </row>
@@ -1137,23 +1137,23 @@
         <v>10791.929283081099</v>
       </c>
       <c r="G16" s="4">
-        <f ca="1">(D16-E16)/F16</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="I16" s="3">
-        <f ca="1">IF(G16&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="K16" t="str">
-        <f ca="1">IF(I16=0, K15, ADDRESS(H16+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$15</v>
       </c>
     </row>
@@ -1180,23 +1180,23 @@
         <v>10791.929283081099</v>
       </c>
       <c r="G17" s="4">
-        <f ca="1">(D17-E17)/F17</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="I17" s="3">
-        <f ca="1">IF(G17&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="K17" t="str">
-        <f ca="1">IF(I17=0, K16, ADDRESS(H17+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$15</v>
       </c>
     </row>
@@ -1223,23 +1223,23 @@
         <v>10791.929283081074</v>
       </c>
       <c r="G18" s="4">
-        <f ca="1">(D18-E18)/F18</f>
+        <f t="shared" ca="1" si="0"/>
         <v>9.1017486507688722E-15</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="I18" s="3">
-        <f ca="1">IF(G18&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="K18" t="str">
-        <f ca="1">IF(I18=0, K17, ADDRESS(H18+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$15</v>
       </c>
     </row>
@@ -1266,23 +1266,23 @@
         <v>10791.929283081059</v>
       </c>
       <c r="G19" s="4">
-        <f ca="1">(D19-E19)/F19</f>
+        <f t="shared" ca="1" si="0"/>
         <v>9.1017486507688849E-15</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="I19" s="3">
-        <f ca="1">IF(G19&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="K19" t="str">
-        <f ca="1">IF(I19=0, K18, ADDRESS(H19+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$15</v>
       </c>
     </row>
@@ -1309,23 +1309,23 @@
         <v>10490.393435568018</v>
       </c>
       <c r="G20" s="4">
-        <f ca="1">(D20-E20)/F20</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0.17246398776084859</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="I20" s="3">
-        <f ca="1">IF(G20&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="K20" t="str">
-        <f ca="1">IF(I20=0, K19, ADDRESS(H20+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$21</v>
       </c>
     </row>
@@ -1352,23 +1352,23 @@
         <v>8982.71419800275</v>
       </c>
       <c r="G21" s="4">
-        <f ca="1">(D21-E21)/F21</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="I21" s="3">
-        <f ca="1">IF(G21&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="K21" t="str">
-        <f ca="1">IF(I21=0, K20, ADDRESS(H21+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$21</v>
       </c>
     </row>
@@ -1395,23 +1395,23 @@
         <v>8982.71419800275</v>
       </c>
       <c r="G22" s="4">
-        <f ca="1">(D22-E22)/F22</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="I22" s="3">
-        <f ca="1">IF(G22&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="K22" t="str">
-        <f ca="1">IF(I22=0, K21, ADDRESS(H22+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$21</v>
       </c>
     </row>
@@ -1438,23 +1438,23 @@
         <v>8982.7133011404931</v>
       </c>
       <c r="G23" s="4">
-        <f ca="1">(D23-E23)/F23</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2.9952940504364824E-7</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="I23" s="3">
-        <f ca="1">IF(G23&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="K23" t="str">
-        <f ca="1">IF(I23=0, K22, ADDRESS(H23+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$21</v>
       </c>
     </row>
@@ -1481,23 +1481,23 @@
         <v>8982.7128527093519</v>
       </c>
       <c r="G24" s="4">
-        <f ca="1">(D24-E24)/F24</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2.9952942546409694E-7</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="I24" s="3">
-        <f ca="1">IF(G24&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="K24" t="str">
-        <f ca="1">IF(I24=0, K23, ADDRESS(H24+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$21</v>
       </c>
     </row>
@@ -1524,23 +1524,23 @@
         <v>8982.7125836506657</v>
       </c>
       <c r="G25" s="4">
-        <f ca="1">(D25-E25)/F25</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2.9952943565087838E-7</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="I25" s="3">
-        <f ca="1">IF(G25&gt;B$2, 1, 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="K25" t="str">
-        <f ca="1">IF(I25=0, K24, ADDRESS(H25+7,3))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>$C$21</v>
       </c>
     </row>
@@ -2609,7 +2609,7 @@
         <v>3</v>
       </c>
       <c r="E49">
-        <f t="shared" ref="E49:O49" si="0">D49+1</f>
+        <f t="shared" ref="E49:G49" si="0">D49+1</f>
         <v>4</v>
       </c>
       <c r="F49">
@@ -2630,23 +2630,23 @@
         <v>384.60553299999998</v>
       </c>
       <c r="C50">
-        <f>B50</f>
+        <f t="shared" ref="C50:D52" si="1">B50</f>
         <v>384.60553299999998</v>
       </c>
       <c r="D50">
-        <f>C50</f>
-        <v>384.60553299999998</v>
-      </c>
-      <c r="E50">
-        <f t="shared" ref="E50:O50" si="1">D50</f>
-        <v>384.60553299999998</v>
-      </c>
-      <c r="F50">
         <f t="shared" si="1"/>
         <v>384.60553299999998</v>
       </c>
+      <c r="E50">
+        <f t="shared" ref="E50:G50" si="2">D50</f>
+        <v>384.60553299999998</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="2"/>
+        <v>384.60553299999998</v>
+      </c>
       <c r="G50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>384.60553299999998</v>
       </c>
     </row>
@@ -2658,23 +2658,23 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <f>B51</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D51">
-        <f>C51</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E51">
-        <f t="shared" ref="E51:O51" si="2">D51</f>
+        <f t="shared" ref="E51:G51" si="3">D51</f>
         <v>1</v>
       </c>
       <c r="F51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2687,23 +2687,23 @@
         <v>7</v>
       </c>
       <c r="C52">
-        <f>B52</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="D52">
-        <f>C52</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E52">
-        <f t="shared" ref="E52:O52" si="3">D52</f>
+        <f t="shared" ref="E52:G52" si="4">D52</f>
         <v>7</v>
       </c>
       <c r="F52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="O52" s="5"/>
@@ -2725,15 +2725,15 @@
         <v>28.465802953499026</v>
       </c>
       <c r="E53">
-        <f t="shared" ref="E53:O53" si="4">D53*D83</f>
+        <f t="shared" ref="E53:G53" si="5">D53*D83</f>
         <v>29.197913116992545</v>
       </c>
       <c r="F53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.440282687604228</v>
       </c>
       <c r="G53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.52004138150614</v>
       </c>
     </row>
@@ -2754,15 +2754,15 @@
         <v>5360239.4927378697</v>
       </c>
       <c r="E54">
-        <f t="shared" ref="E54:O54" si="5">D54</f>
+        <f t="shared" ref="E54:G54" si="6">D54</f>
         <v>5360239.4927378697</v>
       </c>
       <c r="F54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5360239.4927378697</v>
       </c>
       <c r="G54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5360239.4927378697</v>
       </c>
     </row>
@@ -2783,15 +2783,15 @@
         <v>1</v>
       </c>
       <c r="E55">
-        <f t="shared" ref="E55:O55" si="6">D55</f>
+        <f t="shared" ref="E55:G55" si="7">D55</f>
         <v>1</v>
       </c>
       <c r="F55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2812,15 +2812,15 @@
         <v>0.18830452460779742</v>
       </c>
       <c r="E56">
-        <f t="shared" ref="E56:O56" si="7">E54/E53/1000000</f>
+        <f t="shared" ref="E56:G56" si="8">E54/E53/1000000</f>
         <v>0.18358296605856833</v>
       </c>
       <c r="F56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.18207160405408701</v>
       </c>
       <c r="G56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.18157967407511763</v>
       </c>
     </row>
@@ -2833,23 +2833,23 @@
         <v>7</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:K57" si="8">MATCH(C56, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="C57:G57" si="9">MATCH(C56, $A$11:$A$22, 1)</f>
         <v>6</v>
       </c>
       <c r="D57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="E57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="F57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="G57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
@@ -2928,15 +2928,15 @@
         <v>868.63338561378089</v>
       </c>
       <c r="E60">
-        <f t="shared" ref="E60:O60" si="9">E58*E56+E59</f>
+        <f t="shared" ref="E60:G60" si="10">E58*E56+E59</f>
         <v>865.55410829906623</v>
       </c>
       <c r="F60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>864.5684374265785</v>
       </c>
       <c r="G60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>864.24761352725068</v>
       </c>
     </row>
@@ -2956,15 +2956,15 @@
         <v>2</v>
       </c>
       <c r="E61">
-        <f t="shared" ref="E61:O61" si="10">D61</f>
+        <f t="shared" ref="E61:G61" si="11">D61</f>
         <v>2</v>
       </c>
       <c r="F61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="G61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
     </row>
@@ -2985,15 +2985,15 @@
         <v>6</v>
       </c>
       <c r="E62">
-        <f t="shared" ref="E62:O62" si="11">D62</f>
+        <f t="shared" ref="E62:G62" si="12">D62</f>
         <v>6</v>
       </c>
       <c r="F62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="G62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
     </row>
@@ -3014,15 +3014,15 @@
         <v>16.757618295948149</v>
       </c>
       <c r="E63">
-        <f t="shared" ref="E63:O63" si="12">D63*D84</f>
+        <f t="shared" ref="E63:G63" si="13">D63*D84</f>
         <v>16.37203922651252</v>
       </c>
       <c r="F63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>16.231751399709278</v>
       </c>
       <c r="G63">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>16.183401995230348</v>
       </c>
     </row>
@@ -3043,15 +3043,15 @@
         <v>3351880.40539975</v>
       </c>
       <c r="E64">
-        <f t="shared" ref="E64:O64" si="13">D64</f>
+        <f t="shared" ref="E64:G64" si="14">D64</f>
         <v>3351880.40539975</v>
       </c>
       <c r="F64">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3351880.40539975</v>
       </c>
       <c r="G64">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3351880.40539975</v>
       </c>
     </row>
@@ -3072,15 +3072,15 @@
         <v>2</v>
       </c>
       <c r="E65">
-        <f t="shared" ref="E65:O65" si="14">D65</f>
+        <f t="shared" ref="E65:G65" si="15">D65</f>
         <v>2</v>
       </c>
       <c r="F65">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="G65">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
     </row>
@@ -3101,15 +3101,15 @@
         <v>0.20002128859864332</v>
       </c>
       <c r="E66">
-        <f t="shared" ref="E66:O66" si="15">E64/E63/1000000</f>
+        <f t="shared" ref="E66:G66" si="16">E64/E63/1000000</f>
         <v>0.20473200430474101</v>
       </c>
       <c r="F66">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.20650146264929764</v>
       </c>
       <c r="G66">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.20711840479446983</v>
       </c>
     </row>
@@ -3122,23 +3122,23 @@
         <v>5</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67" si="16">MATCH(C66, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="C67" si="17">MATCH(C66, $A$11:$A$22, 1)</f>
         <v>5</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67" si="17">MATCH(D66, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="D67" si="18">MATCH(D66, $A$11:$A$22, 1)</f>
         <v>6</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67" si="18">MATCH(E66, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="E67" si="19">MATCH(E66, $A$11:$A$22, 1)</f>
         <v>6</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67" si="19">MATCH(F66, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="F67" si="20">MATCH(F66, $A$11:$A$22, 1)</f>
         <v>6</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67" si="20">MATCH(G66, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="G67" si="21">MATCH(G66, $A$11:$A$22, 1)</f>
         <v>6</v>
       </c>
     </row>
@@ -3217,15 +3217,15 @@
         <v>856.97137698355675</v>
       </c>
       <c r="E70">
-        <f t="shared" ref="E70:O70" si="21">E68*E66+E69</f>
+        <f t="shared" ref="E70:G70" si="22">E68*E66+E69</f>
         <v>861.4984972942184</v>
       </c>
       <c r="F70">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>863.19899278371338</v>
       </c>
       <c r="G70">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>863.79189023076106</v>
       </c>
     </row>
@@ -3245,15 +3245,15 @@
         <v>3</v>
       </c>
       <c r="E71">
-        <f t="shared" ref="E71:O71" si="22">D71</f>
+        <f t="shared" ref="E71:G71" si="23">D71</f>
         <v>3</v>
       </c>
       <c r="F71">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="G71">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
     </row>
@@ -3274,15 +3274,15 @@
         <v>6</v>
       </c>
       <c r="E72">
-        <f t="shared" ref="E72:O72" si="23">D72</f>
+        <f t="shared" ref="E72:G72" si="24">D72</f>
         <v>6</v>
       </c>
       <c r="F72">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>6</v>
       </c>
       <c r="G72">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>6</v>
       </c>
     </row>
@@ -3303,15 +3303,15 @@
         <v>14.133200424969703</v>
       </c>
       <c r="E73">
-        <f t="shared" ref="E73:O73" si="24">D73*D85</f>
+        <f t="shared" ref="E73:G73" si="25">D73*D85</f>
         <v>13.66465097032953</v>
       </c>
       <c r="F73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>13.522174298085805</v>
       </c>
       <c r="G73">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>13.477471893012513</v>
       </c>
     </row>
@@ -3332,15 +3332,15 @@
         <v>2791240.4248382901</v>
       </c>
       <c r="E74">
-        <f t="shared" ref="E74:O74" si="25">D74</f>
+        <f t="shared" ref="E74:G74" si="26">D74</f>
         <v>2791240.4248382901</v>
       </c>
       <c r="F74">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2791240.4248382901</v>
       </c>
       <c r="G74">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2791240.4248382901</v>
       </c>
     </row>
@@ -3361,15 +3361,15 @@
         <v>2</v>
       </c>
       <c r="E75">
-        <f t="shared" ref="E75:O75" si="26">D75</f>
+        <f t="shared" ref="E75:G75" si="27">D75</f>
         <v>2</v>
       </c>
       <c r="F75">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="G75">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
     </row>
@@ -3390,15 +3390,15 @@
         <v>0.19749528351037121</v>
       </c>
       <c r="E76">
-        <f t="shared" ref="E76:O76" si="27">E74/E73/1000000</f>
+        <f t="shared" ref="E76:G76" si="28">E74/E73/1000000</f>
         <v>0.2042672316255274</v>
       </c>
       <c r="F76">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.20641949758282715</v>
       </c>
       <c r="G76">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.20710415476996302</v>
       </c>
     </row>
@@ -3411,23 +3411,23 @@
         <v>4</v>
       </c>
       <c r="C77">
-        <f t="shared" ref="C77" si="28">MATCH(C76, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="C77" si="29">MATCH(C76, $A$11:$A$22, 1)</f>
         <v>5</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77" si="29">MATCH(D76, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="D77" si="30">MATCH(D76, $A$11:$A$22, 1)</f>
         <v>6</v>
       </c>
       <c r="E77">
-        <f t="shared" ref="E77" si="30">MATCH(E76, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="E77" si="31">MATCH(E76, $A$11:$A$22, 1)</f>
         <v>6</v>
       </c>
       <c r="F77">
-        <f t="shared" ref="F77" si="31">MATCH(F76, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="F77" si="32">MATCH(F76, $A$11:$A$22, 1)</f>
         <v>6</v>
       </c>
       <c r="G77">
-        <f t="shared" ref="G77" si="32">MATCH(G76, $A$11:$A$22, 1)</f>
+        <f t="shared" ref="G77" si="33">MATCH(G76, $A$11:$A$22, 1)</f>
         <v>6</v>
       </c>
     </row>
@@ -3506,15 +3506,15 @@
         <v>854.54382039695372</v>
       </c>
       <c r="E80">
-        <f t="shared" ref="E80:O80" si="33">E78*E76+E79</f>
+        <f t="shared" ref="E80:G80" si="34">E78*E76+E79</f>
         <v>861.05183866160667</v>
       </c>
       <c r="F80">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>863.12022222307382</v>
       </c>
       <c r="G80">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>863.7781955865928</v>
       </c>
     </row>
@@ -3535,15 +3535,15 @@
         <v>862.47812099413056</v>
       </c>
       <c r="E82">
-        <f t="shared" ref="E82:O82" si="34">(E80*E73*E72+E70*E63*E62+E60*E53*E52)/(E73*E72+E63*E62+E53*E52)</f>
+        <f t="shared" ref="E82:G82" si="35">(E80*E73*E72+E70*E63*E62+E60*E53*E52)/(E73*E72+E63*E62+E53*E52)</f>
         <v>863.55849635924983</v>
       </c>
       <c r="F82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>863.91616126598183</v>
       </c>
       <c r="G82">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>864.03386121380731</v>
       </c>
     </row>
@@ -3564,15 +3564,15 @@
         <v>1.0257189359699241</v>
       </c>
       <c r="E83">
-        <f t="shared" ref="E83:O83" si="35">(E60-623.15)/(E82-623.15)</f>
+        <f t="shared" ref="E83:G83" si="36">(E60-623.15)/(E82-623.15)</f>
         <v>1.0083009210158458</v>
       </c>
       <c r="F83">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0027091687518168</v>
       </c>
       <c r="G83">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.0008873666851996</v>
       </c>
     </row>
@@ -3593,15 +3593,15 @@
         <v>0.9769908191828871</v>
       </c>
       <c r="E84">
-        <f t="shared" ref="E84:O84" si="36">(E70-623.15)/(E82-623.15)</f>
+        <f t="shared" ref="E84:G84" si="37">(E70-623.15)/(E82-623.15)</f>
         <v>0.99143125515017938</v>
       </c>
       <c r="F84">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.99702130698725489</v>
       </c>
       <c r="G84">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.99899548694616991</v>
       </c>
     </row>
@@ -3622,15 +3622,15 @@
         <v>0.96684760418366622</v>
       </c>
       <c r="E85">
-        <f t="shared" ref="E85:O85" si="37">(E80-623.15)/(E82-623.15)</f>
+        <f t="shared" ref="E85:G85" si="38">(E80-623.15)/(E82-623.15)</f>
         <v>0.98957333981284346</v>
       </c>
       <c r="F85">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.99669414074335516</v>
       </c>
       <c r="G85">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.99893863529949156</v>
       </c>
     </row>
@@ -3651,15 +3651,15 @@
         <v>11.452713132802657</v>
       </c>
       <c r="E87">
-        <f t="shared" ref="E87:O87" si="38">SQRT((E60-E82)^2+(E70-E82)^2+(E80-E82)^2)</f>
+        <f t="shared" ref="E87:G87" si="39">SQRT((E60-E82)^2+(E70-E82)^2+(E80-E82)^2)</f>
         <v>3.8091201051452654</v>
       </c>
       <c r="F87">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>1.2543180544292869</v>
       </c>
       <c r="G87">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.41183118031270138</v>
       </c>
     </row>
@@ -3680,15 +3680,15 @@
         <v>0</v>
       </c>
       <c r="E88">
-        <f t="shared" ref="E88:O88" si="39">IF(E87&lt;1, 1, 0)</f>
+        <f t="shared" ref="E88:G88" si="40">IF(E87&lt;1, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="F88">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="G88">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
         <v>3</v>
       </c>
       <c r="E75">
-        <f t="shared" ref="E75:O75" si="2">D75+1</f>
+        <f t="shared" ref="E75:G75" si="2">D75+1</f>
         <v>4</v>
       </c>
       <c r="F75">
@@ -5490,23 +5490,23 @@
         <v>383.01455710961341</v>
       </c>
       <c r="C76">
-        <f>B76</f>
+        <f t="shared" ref="C76:D78" si="3">B76</f>
         <v>383.01455710961341</v>
       </c>
       <c r="D76">
-        <f>C76</f>
-        <v>383.01455710961341</v>
-      </c>
-      <c r="E76">
-        <f t="shared" ref="E76:O76" si="3">D76</f>
-        <v>383.01455710961341</v>
-      </c>
-      <c r="F76">
         <f t="shared" si="3"/>
         <v>383.01455710961341</v>
       </c>
+      <c r="E76">
+        <f t="shared" ref="E76:G76" si="4">D76</f>
+        <v>383.01455710961341</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="4"/>
+        <v>383.01455710961341</v>
+      </c>
       <c r="G76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>383.01455710961341</v>
       </c>
     </row>
@@ -5518,23 +5518,23 @@
         <v>1</v>
       </c>
       <c r="C77">
-        <f>B77</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D77">
-        <f>C77</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E77">
-        <f t="shared" ref="E77:O77" si="4">D77</f>
+        <f t="shared" ref="E77:G77" si="5">D77</f>
         <v>1</v>
       </c>
       <c r="F77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -5547,23 +5547,23 @@
         <v>7</v>
       </c>
       <c r="C78">
-        <f>B78</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="D78">
-        <f>C78</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="E78">
-        <f t="shared" ref="E78:O78" si="5">D78</f>
+        <f t="shared" ref="E78:G78" si="6">D78</f>
         <v>7</v>
       </c>
       <c r="F78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="G78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
     </row>
@@ -5584,15 +5584,15 @@
         <v>29.193109048201858</v>
       </c>
       <c r="E79">
-        <f t="shared" ref="E79:O79" si="6">D79*D112</f>
+        <f t="shared" ref="E79:G79" si="7">D79*D112</f>
         <v>29.985575767726793</v>
       </c>
       <c r="F79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30.244611963140066</v>
       </c>
       <c r="G79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30.328698694369983</v>
       </c>
     </row>
@@ -5613,15 +5613,15 @@
         <v>5360239.4927378697</v>
       </c>
       <c r="E80">
-        <f t="shared" ref="E80:O80" si="7">D80</f>
+        <f t="shared" ref="E80:G80" si="8">D80</f>
         <v>5360239.4927378697</v>
       </c>
       <c r="F80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5360239.4927378697</v>
       </c>
       <c r="G80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5360239.4927378697</v>
       </c>
     </row>
@@ -5642,15 +5642,15 @@
         <v>1</v>
       </c>
       <c r="E81">
-        <f t="shared" ref="E81:O81" si="8">D81</f>
+        <f t="shared" ref="E81:G81" si="9">D81</f>
         <v>1</v>
       </c>
       <c r="F81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="G81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -5671,15 +5671,15 @@
         <v>0.18361317679070679</v>
       </c>
       <c r="E82">
-        <f t="shared" ref="E82:O82" si="9">E80/E79/1000000</f>
+        <f t="shared" ref="E82:G82" si="10">E80/E79/1000000</f>
         <v>0.1787605992380859</v>
       </c>
       <c r="F82">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.17722956734477333</v>
       </c>
       <c r="G82">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.1767381959494658</v>
       </c>
     </row>
@@ -5700,15 +5700,15 @@
         <v>5</v>
       </c>
       <c r="E83">
-        <f t="shared" ref="E83:O83" si="10">MATCH(E82, $A$37:$A$48, 1)</f>
+        <f t="shared" ref="E83:G83" si="11">MATCH(E82, $A$37:$A$48, 1)</f>
         <v>5</v>
       </c>
       <c r="F83">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="G83">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
     </row>
@@ -5787,15 +5787,15 @@
         <v>1.0100331516719059</v>
       </c>
       <c r="E86">
-        <f t="shared" ref="E86:O86" si="11">D86</f>
+        <f t="shared" ref="E86:G86" si="12">D86</f>
         <v>1.0100331516719059</v>
       </c>
       <c r="F86">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.0100331516719059</v>
       </c>
       <c r="G86">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.0100331516719059</v>
       </c>
     </row>
@@ -5816,15 +5816,15 @@
         <v>874.25824427895645</v>
       </c>
       <c r="E87">
-        <f t="shared" ref="E87:O87" si="12">(E84*E82+E85)*E86</f>
+        <f t="shared" ref="E87:G87" si="13">(E84*E82+E85)*E86</f>
         <v>871.06176762730036</v>
       </c>
       <c r="F87">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>870.0532504739225</v>
       </c>
       <c r="G87">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>869.7295756484591</v>
       </c>
     </row>
@@ -5844,15 +5844,15 @@
         <v>2</v>
       </c>
       <c r="E88">
-        <f t="shared" ref="E88:O88" si="13">D88</f>
+        <f t="shared" ref="E88:G88" si="14">D88</f>
         <v>2</v>
       </c>
       <c r="F88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="G88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
     </row>
@@ -5873,15 +5873,15 @@
         <v>6</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89:O89" si="14">D89</f>
+        <f t="shared" ref="E89:G89" si="15">D89</f>
         <v>6</v>
       </c>
       <c r="F89">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="G89">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
     </row>
@@ -5902,15 +5902,15 @@
         <v>16.19683529721506</v>
       </c>
       <c r="E90">
-        <f t="shared" ref="E90:O90" si="15">D90*D113</f>
+        <f t="shared" ref="E90:G90" si="16">D90*D113</f>
         <v>15.76068593443679</v>
       </c>
       <c r="F90">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>15.605986171580923</v>
       </c>
       <c r="G90">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>15.553833916190634</v>
       </c>
     </row>
@@ -5931,15 +5931,15 @@
         <v>3351880.40539975</v>
       </c>
       <c r="E91">
-        <f t="shared" ref="E91:O91" si="16">D91</f>
+        <f t="shared" ref="E91:G91" si="17">D91</f>
         <v>3351880.40539975</v>
       </c>
       <c r="F91">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3351880.40539975</v>
       </c>
       <c r="G91">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3351880.40539975</v>
       </c>
     </row>
@@ -5960,15 +5960,15 @@
         <v>2</v>
       </c>
       <c r="E92">
-        <f t="shared" ref="E92:O92" si="17">D92</f>
+        <f t="shared" ref="E92:G92" si="18">D92</f>
         <v>2</v>
       </c>
       <c r="F92">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="G92">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
     </row>
@@ -5989,15 +5989,15 @@
         <v>0.20694662530624633</v>
       </c>
       <c r="E93">
-        <f t="shared" ref="E93:O93" si="18">E91/E90/1000000</f>
+        <f t="shared" ref="E93:G93" si="19">E91/E90/1000000</f>
         <v>0.21267351048953759</v>
       </c>
       <c r="F93">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.21478171059151954</v>
       </c>
       <c r="G93">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.21550187712308269</v>
       </c>
     </row>
@@ -6018,15 +6018,15 @@
         <v>6</v>
       </c>
       <c r="E94">
-        <f t="shared" ref="E94:O94" si="19">MATCH(E93, $A$37:$A$48, 1)</f>
+        <f t="shared" ref="E94:G94" si="20">MATCH(E93, $A$37:$A$48, 1)</f>
         <v>6</v>
       </c>
       <c r="F94">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>6</v>
       </c>
       <c r="G94">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>6</v>
       </c>
     </row>
@@ -6105,15 +6105,15 @@
         <v>0.99700325387808175</v>
       </c>
       <c r="E97">
-        <f t="shared" ref="E97:O97" si="20">D97</f>
+        <f t="shared" ref="E97:G97" si="21">D97</f>
         <v>0.99700325387808175</v>
       </c>
       <c r="F97">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.99700325387808175</v>
       </c>
       <c r="G97">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.99700325387808175</v>
       </c>
     </row>
@@ -6134,15 +6134,15 @@
         <v>861.03873539421693</v>
       </c>
       <c r="E98">
-        <f t="shared" ref="E98:O98" si="21">(E95*E93+E96)*E97</f>
+        <f t="shared" ref="E98:G98" si="22">(E95*E93+E96)*E97</f>
         <v>866.52592785267268</v>
       </c>
       <c r="F98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>868.54589146819319</v>
       </c>
       <c r="G98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>869.23591619094384</v>
       </c>
     </row>
@@ -6162,15 +6162,15 @@
         <v>3</v>
       </c>
       <c r="E99">
-        <f t="shared" ref="E99:O99" si="22">D99</f>
+        <f t="shared" ref="E99:G99" si="23">D99</f>
         <v>3</v>
       </c>
       <c r="F99">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="G99">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
     </row>
@@ -6191,15 +6191,15 @@
         <v>6</v>
       </c>
       <c r="E100">
-        <f t="shared" ref="E100:O100" si="23">D100</f>
+        <f t="shared" ref="E100:G100" si="24">D100</f>
         <v>6</v>
       </c>
       <c r="F100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>6</v>
       </c>
       <c r="G100">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>6</v>
       </c>
     </row>
@@ -6220,15 +6220,15 @@
         <v>13.580296998151683</v>
       </c>
       <c r="E101">
-        <f t="shared" ref="E101:O101" si="24">D101*D114</f>
+        <f t="shared" ref="E101:G101" si="25">D101*D114</f>
         <v>13.09190185481758</v>
       </c>
       <c r="F101">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>12.944392723024606</v>
       </c>
       <c r="G101">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>12.898443791979981</v>
       </c>
     </row>
@@ -6249,15 +6249,15 @@
         <v>2791240.4248382901</v>
       </c>
       <c r="E102">
-        <f t="shared" ref="E102:O102" si="25">D102</f>
+        <f t="shared" ref="E102:G102" si="26">D102</f>
         <v>2791240.4248382901</v>
       </c>
       <c r="F102">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2791240.4248382901</v>
       </c>
       <c r="G102">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2791240.4248382901</v>
       </c>
     </row>
@@ -6278,15 +6278,15 @@
         <v>2</v>
       </c>
       <c r="E103">
-        <f t="shared" ref="E103:O103" si="26">D103</f>
+        <f t="shared" ref="E103:G103" si="27">D103</f>
         <v>2</v>
       </c>
       <c r="F103">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="G103">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
     </row>
@@ -6307,15 +6307,15 @@
         <v>0.20553603689361036</v>
       </c>
       <c r="E104">
-        <f t="shared" ref="E104:O104" si="27">E102/E101/1000000</f>
+        <f t="shared" ref="E104:G104" si="28">E102/E101/1000000</f>
         <v>0.21320358613986742</v>
       </c>
       <c r="F104">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.21563316909208274</v>
       </c>
       <c r="G104">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.21640133258353486</v>
       </c>
     </row>
@@ -6336,15 +6336,15 @@
         <v>6</v>
       </c>
       <c r="E105">
-        <f t="shared" ref="E105:O105" si="28">MATCH(E104, $A$37:$A$48, 1)</f>
+        <f t="shared" ref="E105:G105" si="29">MATCH(E104, $A$37:$A$48, 1)</f>
         <v>6</v>
       </c>
       <c r="F105">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
       <c r="G105">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>6</v>
       </c>
     </row>
@@ -6423,15 +6423,15 @@
         <v>0.9960089453636608</v>
       </c>
       <c r="E108">
-        <f t="shared" ref="E108:O108" si="29">D108</f>
+        <f t="shared" ref="E108:G108" si="30">D108</f>
         <v>0.9960089453636608</v>
       </c>
       <c r="F108">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.9960089453636608</v>
       </c>
       <c r="G108">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.9960089453636608</v>
       </c>
     </row>
@@ -6452,15 +6452,15 @@
         <v>858.8298220788455</v>
       </c>
       <c r="E109">
-        <f t="shared" ref="E109:O109" si="30">(E106*E104+E107)*E108</f>
+        <f t="shared" ref="E109:G109" si="31">(E106*E104+E107)*E108</f>
         <v>866.16912738228439</v>
       </c>
       <c r="F109">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>868.49470110521077</v>
       </c>
       <c r="G109">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>869.22997990234057</v>
       </c>
     </row>
@@ -6481,15 +6481,15 @@
         <v>867.62188924842917</v>
       </c>
       <c r="E111">
-        <f t="shared" ref="E111:O111" si="31">(E109*E101*E100+E98*E90*E89+E87*E79*E78)/(E101*E100+E90*E89+E79*E78)</f>
+        <f t="shared" ref="E111:G111" si="32">(E109*E101*E100+E98*E90*E89+E87*E79*E78)/(E101*E100+E90*E89+E79*E78)</f>
         <v>868.93847633949611</v>
       </c>
       <c r="F111">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>869.36870784083396</v>
       </c>
       <c r="G111">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>869.50834690504098</v>
       </c>
     </row>
@@ -6510,15 +6510,15 @@
         <v>1.0271456773657257</v>
       </c>
       <c r="E112">
-        <f t="shared" ref="E112:O112" si="32">(E87-623.15)/(E111-623.15)</f>
+        <f t="shared" ref="E112:G112" si="33">(E87-623.15)/(E111-623.15)</f>
         <v>1.0086386933977793</v>
       </c>
       <c r="F112">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.0027802218567854</v>
       </c>
       <c r="G112">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.0008979957293811</v>
       </c>
     </row>
@@ -6539,15 +6539,15 @@
         <v>0.97307193937736325</v>
       </c>
       <c r="E113">
-        <f t="shared" ref="E113:O113" si="33">(E98-623.15)/(E111-623.15)</f>
+        <f t="shared" ref="E113:G113" si="34">(E98-623.15)/(E111-623.15)</f>
         <v>0.99018445240902553</v>
       </c>
       <c r="F113">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.9966581890553472</v>
       </c>
       <c r="G113">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.99889416893107275</v>
       </c>
     </row>
@@ -6568,15 +6568,15 @@
         <v>0.96403649026228411</v>
       </c>
       <c r="E114">
-        <f t="shared" ref="E114:O114" si="34">(E109-623.15)/(E111-623.15)</f>
+        <f t="shared" ref="E114:G114" si="35">(E109-623.15)/(E111-623.15)</f>
         <v>0.98873279578255513</v>
       </c>
       <c r="F114">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.99645028298910499</v>
       </c>
       <c r="G114">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.99887007277732831</v>
       </c>
     </row>
@@ -6597,15 +6597,15 @@
         <v>12.83275371359964</v>
       </c>
       <c r="E116">
-        <f t="shared" ref="E116:O116" si="35">SQRT((E87-E111)^2+(E98-E111)^2+(E109-E111)^2)</f>
+        <f t="shared" ref="E116:G116" si="36">SQRT((E87-E111)^2+(E98-E111)^2+(E109-E111)^2)</f>
         <v>4.2424108406599501</v>
       </c>
       <c r="F116">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.3818513572436903</v>
       </c>
       <c r="G116">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.44793843225408542</v>
       </c>
     </row>
@@ -6626,15 +6626,15 @@
         <v>0</v>
       </c>
       <c r="E117">
-        <f t="shared" ref="E117:O117" si="36">IF(E116&lt;1, 1, 0)</f>
+        <f t="shared" ref="E117:G117" si="37">IF(E116&lt;1, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="F117">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="G117">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
     </row>
@@ -6648,10 +6648,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FAE111-94F8-664F-8FDD-52DC2691C30F}">
-  <dimension ref="A1:O117"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7236,490 +7236,6 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="6"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="3"/>
-      <c r="J53" s="6"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="3"/>
-      <c r="J54" s="6"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="3"/>
-      <c r="J55" s="6"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="3"/>
-      <c r="J56" s="6"/>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="3"/>
-      <c r="J57" s="6"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="3"/>
-      <c r="J58" s="6"/>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="3"/>
-      <c r="J59" s="6"/>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="3"/>
-      <c r="J60" s="6"/>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="3"/>
-      <c r="J61" s="6"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="3"/>
-      <c r="J62" s="6"/>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="3"/>
-      <c r="J63" s="6"/>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="3"/>
-      <c r="J64" s="6"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7"/>
-      <c r="H65" s="3"/>
-      <c r="J65" s="6"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="3"/>
-      <c r="J66" s="6"/>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="3"/>
-      <c r="J67" s="6"/>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="3"/>
-      <c r="J68" s="6"/>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="3"/>
-      <c r="J69" s="6"/>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="3"/>
-      <c r="J70" s="6"/>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="3"/>
-      <c r="J71" s="6"/>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B79" s="11"/>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B80" s="8"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="8"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="8"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="8"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="8"/>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="9"/>
-      <c r="B88" s="9"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="9"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B90" s="11"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B91" s="8"/>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="8"/>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="8"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="8"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="8"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="8"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="8"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="9"/>
-      <c r="B99" s="9"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="9"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B101" s="11"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="8"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="8"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="8"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="8"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="8"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="8"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="8"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>51</v>
-      </c>
-      <c r="B116">
-        <f>SQRT((B87-B111)^2+(B98-B111)^2+(B109-B111)^2)</f>
-        <v>0</v>
-      </c>
-      <c r="C116">
-        <f>SQRT((C87-C111)^2+(C98-C111)^2+(C109-C111)^2)</f>
-        <v>0</v>
-      </c>
-      <c r="D116">
-        <f>SQRT((D87-D111)^2+(D98-D111)^2+(D109-D111)^2)</f>
-        <v>0</v>
-      </c>
-      <c r="E116">
-        <f t="shared" ref="E116:O116" si="1">SQRT((E87-E111)^2+(E98-E111)^2+(E109-E111)^2)</f>
-        <v>0</v>
-      </c>
-      <c r="F116">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G116">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>52</v>
-      </c>
-      <c r="B117">
-        <f>IF(B116&lt;1, 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="C117">
-        <f>IF(C116&lt;1, 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="D117">
-        <f>IF(D116&lt;1, 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="E117">
-        <f t="shared" ref="E117:G117" si="2">IF(E116&lt;1, 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="F117">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G117">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>